<commit_message>
error list and discription added
</commit_message>
<xml_diff>
--- a/QA/Property_Booking_Bug_list.xlsx
+++ b/QA/Property_Booking_Bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Bug Description</t>
   </si>
@@ -43,16 +43,106 @@
   </si>
   <si>
     <t>Developer comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Unable to login after searching for rooms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Login window is distorted.</t>
+  </si>
+  <si>
+    <t>Snehal</t>
+  </si>
+  <si>
+    <t>Unable to login with admin/admin</t>
+  </si>
+  <si>
+    <t>Shruti</t>
+  </si>
+  <si>
+    <t>Sujay Sir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              9/2/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               9/2/2016</t>
+  </si>
+  <si>
+    <t>Validation on search is still pending. Still able to search using past dates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Every search result shows 2 unwanted texts as shown below. This text is shown with or without any results. They are no hyperlinks or linked with any property. Remove them
+    $4,650 $2,650
+    Best price
+</t>
+  </si>
+  <si>
+    <t>Search filters are not aligned properly. Each search section must same height for title. Reduce height for all headers in like Name contains, Per night rate, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check boxes shown in search filters must also have equal spacing. For Star rating there is spacing between check box and rating. But for Features, there is no spacing. Reduce spacing and height of each Star rating sections check box. Same height and spacing must be given to all filter options.
+</t>
+  </si>
+  <si>
+    <t>Mukesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Facilites Filter section -
+    a. There is additional dot before "Accomodation type".
+    b. Accomodation type is shown with collapsible link, on click nothing happens.
+    c. Options must be shwon as check boxes instead of links. This way user can select/deselect a option. Make sure same style is applied for all sections.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on "Continue" : nothing happens - http://propertybook.agilesoftsol.com/single.html
+</t>
+  </si>
+  <si>
+    <t>After I open a property from property search, i see name of vishwanath at the end of the page without any context. Like is open "Vg Homes".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Send mail form
+    a. Form have  too much spacing.
+    b. Label and fields are not aligned
+    c. Date fields doesnt show popup in aligned with field.
+    d. Unable to select date.
+    e. Show a bigger Enquiry text area.
+    f. Weired message alert is shown on send button - "from here it will get to piyu mney"</t>
+  </si>
+  <si>
+    <t>Mukesh/Shruti</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Send SMS
+    a. Form have  too much spacing.
+    b. Label and fields are not aligned
+    c. Title of the popup should be "Send SMS" instead of "Enquiry via email"
+    d. Weired message alert is shown on send button - "from here it will get to piyu mney"
+</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Due to change in CSS it was distorted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,8 +168,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,21 +469,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I2"/>
+  <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9">
@@ -420,8 +517,228 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:9" ht="15.75">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>42615</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="105">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="120">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="150">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2">
+        <v>42615</v>
+      </c>
+      <c r="G12" s="2">
+        <v>42615</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="135">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2">
+        <v>42615</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="120">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2">
+        <v>42615</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
- updated End Date against each Bug
</commit_message>
<xml_diff>
--- a/QA/Property_Booking_Bug_list.xlsx
+++ b/QA/Property_Booking_Bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Bug Description</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Due to change in CSS it was distorted</t>
+  </si>
+  <si>
+    <t>Shruti/Mukesh</t>
   </si>
 </sst>
 </file>
@@ -471,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15"/>
@@ -533,6 +536,9 @@
       <c r="F3" s="2">
         <v>42615</v>
       </c>
+      <c r="G3" s="2">
+        <v>42645</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="30">
       <c r="A4">
@@ -576,6 +582,9 @@
       <c r="F5" s="2">
         <v>42615</v>
       </c>
+      <c r="G5" s="2">
+        <v>42645</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="30">
       <c r="A6">
@@ -593,6 +602,9 @@
       <c r="F6" t="s">
         <v>16</v>
       </c>
+      <c r="G6" s="2">
+        <v>42676</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="105">
       <c r="A7">
@@ -610,6 +622,9 @@
       <c r="F7" s="2">
         <v>42615</v>
       </c>
+      <c r="G7" s="2">
+        <v>42615</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="60">
       <c r="A8">
@@ -619,13 +634,16 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="2">
         <v>42615</v>
+      </c>
+      <c r="G8" s="2">
+        <v>42645</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="120">
@@ -644,6 +662,9 @@
       <c r="F9" s="2">
         <v>42615</v>
       </c>
+      <c r="G9" s="2">
+        <v>42645</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="150">
       <c r="A10">
@@ -661,6 +682,9 @@
       <c r="F10" s="2">
         <v>42615</v>
       </c>
+      <c r="G10" s="2">
+        <v>42676</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="60">
       <c r="A11">
@@ -678,6 +702,9 @@
       <c r="F11" s="2">
         <v>42615</v>
       </c>
+      <c r="G11" s="2">
+        <v>42706</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="60">
       <c r="A12">
@@ -718,6 +745,9 @@
       <c r="F13" s="2">
         <v>42615</v>
       </c>
+      <c r="G13" s="2">
+        <v>42645</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="120">
       <c r="A14">
@@ -734,6 +764,9 @@
       </c>
       <c r="F14" s="2">
         <v>42615</v>
+      </c>
+      <c r="G14" s="2">
+        <v>42645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assigned task to mukesh
</commit_message>
<xml_diff>
--- a/QA/Property_Booking_Bug_list.xlsx
+++ b/QA/Property_Booking_Bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Bug Description</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Resolved</t>
-  </si>
-  <si>
-    <t>Due to change in CSS it was distorted</t>
   </si>
   <si>
     <t>Shruti/Mukesh</t>
@@ -474,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15"/>
@@ -540,7 +537,7 @@
         <v>42645</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
@@ -548,7 +545,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -559,12 +556,7 @@
       <c r="G4" s="2">
         <v>42615</v>
       </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
       <c r="A5">
@@ -585,6 +577,9 @@
       <c r="G5" s="2">
         <v>42645</v>
       </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="30">
       <c r="A6">
@@ -634,7 +629,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
added menu.html and meusController.js file updated index.html for menus.html
</commit_message>
<xml_diff>
--- a/QA/Property_Booking_Bug_list.xlsx
+++ b/QA/Property_Booking_Bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Bug Description</t>
   </si>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15"/>
@@ -536,6 +536,9 @@
       <c r="G3" s="2">
         <v>42645</v>
       </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
@@ -555,6 +558,9 @@
       </c>
       <c r="G4" s="2">
         <v>42615</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
       </c>
       <c r="I4" s="3"/>
     </row>

</xml_diff>

<commit_message>
st4eps for debugging code explains flow
</commit_message>
<xml_diff>
--- a/QA/Property_Booking_Bug_list.xlsx
+++ b/QA/Property_Booking_Bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Bug Description</t>
   </si>
@@ -111,6 +111,9 @@
     f. Weired message alert is shown on send button - "from here it will get to piyu mney"</t>
   </si>
   <si>
+    <t>Mukesh/Shruti</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Send SMS
     a. Form have  too much spacing.
     b. Label and fields are not aligned
@@ -123,31 +126,6 @@
   </si>
   <si>
     <t>Shruti/Mukesh</t>
-  </si>
-  <si>
-    <t>Snehal/Mukesh</t>
-  </si>
-  <si>
-    <t>1. In property search page - when i select any check box, i get alert - "Message sent succesfully". Remove such development messages in SVN</t>
-  </si>
-  <si>
-    <t>15/2/2016</t>
-  </si>
-  <si>
-    <t>Accomodations name must be proper - 1bhk should be 1 BHK</t>
-  </si>
-  <si>
-    <t>Reduce the height and spacing of Star rating. Taking a bit more space.</t>
-  </si>
-  <si>
-    <t>Make all Sections expanded at same time
- currently only one section can be seen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> On home page Search bar is shown after the image instead of above.Also it is not changing the look and feel to original needs</t>
-  </si>
-  <si>
-    <t>Reduce the height of first 4 sections shown in property search</t>
   </si>
 </sst>
 </file>
@@ -190,14 +168,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I20"/>
+  <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15"/>
@@ -559,9 +536,6 @@
       <c r="G3" s="2">
         <v>42645</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
@@ -582,9 +556,6 @@
       <c r="G4" s="2">
         <v>42615</v>
       </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
@@ -607,7 +578,7 @@
         <v>42645</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30">
@@ -649,9 +620,6 @@
       <c r="G7" s="2">
         <v>42615</v>
       </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="8" spans="1:9" ht="60">
       <c r="A8">
@@ -661,7 +629,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -701,7 +669,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -711,9 +679,6 @@
       </c>
       <c r="G10" s="2">
         <v>42676</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60">
@@ -724,7 +689,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -734,9 +699,6 @@
       </c>
       <c r="G11" s="2">
         <v>42706</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="60">
@@ -747,7 +709,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -759,7 +721,7 @@
         <v>42615</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="135">
@@ -770,7 +732,7 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -787,10 +749,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -800,126 +762,6 @@
       </c>
       <c r="G14" s="2">
         <v>42645</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="60">
-      <c r="A15" s="3">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45">
-      <c r="A19" s="4">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30">
-      <c r="A20" s="4">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated js controller files to solve bugs ,QA list is updated
</commit_message>
<xml_diff>
--- a/QA/Property_Booking_Bug_list.xlsx
+++ b/QA/Property_Booking_Bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>Bug Description</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Reduce the height of first 4 sections shown in property search</t>
+  </si>
+  <si>
+    <t>Resolved e,f</t>
+  </si>
+  <si>
+    <t>Resolved c,d</t>
   </si>
 </sst>
 </file>
@@ -494,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15"/>
@@ -692,6 +698,9 @@
       <c r="G9" s="2">
         <v>42645</v>
       </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="150">
       <c r="A10">
@@ -770,7 +779,7 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -780,6 +789,9 @@
       </c>
       <c r="G13" s="2">
         <v>42645</v>
+      </c>
+      <c r="H13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="120">
@@ -801,6 +813,9 @@
       <c r="G14" s="2">
         <v>42645</v>
       </c>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="60">
       <c r="A15" s="3">
@@ -821,6 +836,9 @@
       <c r="G15" t="s">
         <v>31</v>
       </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="30">
       <c r="A16">
@@ -840,6 +858,9 @@
       </c>
       <c r="G16" t="s">
         <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30">

</xml_diff>

<commit_message>
updated getRoomDetailController.js,search.html and contact.php file for sendsms and send email popup code.updated QA list
</commit_message>
<xml_diff>
--- a/QA/Property_Booking_Bug_list.xlsx
+++ b/QA/Property_Booking_Bug_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>Bug Description</t>
   </si>
@@ -150,10 +150,10 @@
     <t>Reduce the height of first 4 sections shown in property search</t>
   </si>
   <si>
-    <t>Resolved e,f</t>
-  </si>
-  <si>
     <t>Resolved c,d</t>
+  </si>
+  <si>
+    <t>Resolved c,d,e,f</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15"/>
@@ -767,7 +767,7 @@
       <c r="G12" s="2">
         <v>42615</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -790,8 +790,8 @@
       <c r="G13" s="2">
         <v>42645</v>
       </c>
-      <c r="H13" t="s">
-        <v>37</v>
+      <c r="H13" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="120">
@@ -814,7 +814,7 @@
         <v>42645</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60">
@@ -863,7 +863,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30">
+    <row r="17" spans="1:8" ht="30">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -883,7 +883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:8" ht="30">
       <c r="A18">
         <v>16</v>
       </c>
@@ -903,7 +903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45">
+    <row r="19" spans="1:8" ht="45">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -922,8 +922,11 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="30">
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30">
       <c r="A20" s="4">
         <v>18</v>
       </c>

</xml_diff>